<commit_message>
File umbenannt und Sprint Review 1 Prorokoll erweitert
</commit_message>
<xml_diff>
--- a/Org/Sprint_Review_Protocol1.xlsx
+++ b/Org/Sprint_Review_Protocol1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Studium\FHTechnikumWien\3. Semester\9_InnovationLab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Studium\FHTechnikumWien\3. Semester\9_InnovationLab\LocalRep\Org\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Get To Know Unity</t>
+  </si>
+  <si>
+    <t>Alle Teammitglieder beschäftigen sich mit Unity, führen Installation durch</t>
+  </si>
+  <si>
+    <t>Es sollen existierende Lösungen rund um DICOM Import gesucht werden</t>
+  </si>
+  <si>
+    <t>Passende Codes rund um DICOM import sollen getestet werden, optimalerweise wird dadurch klar, mit welcher weitergearbeitet wird</t>
   </si>
 </sst>
 </file>
@@ -379,17 +388,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -397,50 +412,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,47 +767,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" style="2"/>
-    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="84.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -809,11 +818,11 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="18">
         <v>1</v>
       </c>
@@ -822,123 +831,123 @@
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="30">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20">
         <v>41948</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="20">
+      <c r="B6" s="17"/>
+      <c r="C6" s="21">
         <v>16</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -964,7 +973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -983,9 +992,11 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -1004,9 +1015,11 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -1025,9 +1038,11 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -1042,7 +1057,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5</v>
       </c>
@@ -1057,7 +1072,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>6</v>
       </c>
@@ -1072,7 +1087,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>7</v>
       </c>
@@ -1087,7 +1102,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1117,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -1117,7 +1132,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1147,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f>COUNT(A16:A25)</f>
         <v>7</v>
@@ -1154,19 +1169,23 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
@@ -1183,10 +1202,6 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mitschrift von Review hinzugefuegt
</commit_message>
<xml_diff>
--- a/Org/Sprint_Review_Protocol1.xlsx
+++ b/Org/Sprint_Review_Protocol1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Passende Codes rund um DICOM import sollen getestet werden, optimalerweise wird dadurch klar, mit welcher weitergearbeitet wird</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -388,6 +391,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -406,12 +427,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,18 +453,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,7 +771,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -784,28 +787,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -819,133 +822,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18">
+      <c r="B4" s="21"/>
+      <c r="C4" s="22">
         <v>1</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20">
+      <c r="B5" s="13"/>
+      <c r="C5" s="24">
         <v>41948</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="21">
+      <c r="B6" s="13"/>
+      <c r="C6" s="25">
         <v>16</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -990,7 +993,9 @@
         <f>D16-C16</f>
         <v>-1</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="7" t="s">
         <v>33</v>
@@ -1013,7 +1018,9 @@
         <f t="shared" ref="E17:E25" si="0">D17-C17</f>
         <v>10</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="7" t="s">
         <v>34</v>
@@ -1036,7 +1043,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="7" t="s">
         <v>32</v>
@@ -1182,11 +1191,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1201,6 +1205,11 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>